<commit_message>
perbaikan load excel, tampil count, env jadi txt
</commit_message>
<xml_diff>
--- a/queries/query_list.xlsx
+++ b/queries/query_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2025\SERUTI\evaluasi-seruti-1800\queries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B213A0-AF21-4FBD-B8BD-C9E9CD78EFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7065261-9CD8-4644-893D-D8FE1609777E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{764EDEE2-3088-4AC6-90FD-CA006F98D4D8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>id</t>
   </si>
@@ -229,7 +229,37 @@
     <t>Ada ART usia sekolah tetapi tidak ada pengeluaran terkait pendidikan (R456K3)</t>
   </si>
   <si>
-    <t>SELECT ROW_NUMBER() OVER (ORDER BY id_inti) AS no_urut, id_inti, R456K3, jml_art_usia_sekolah,Catatan from inti_rt i 
+    <t>t2</t>
+  </si>
+  <si>
+    <t>T2. Rincian Lainnya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rincian 'Lainnya' di kuesioner makanan </t>
+  </si>
+  <si>
+    <t>tabel</t>
+  </si>
+  <si>
+    <t>SELECT 
+    ROW_NUMBER() OVER (ORDER BY id_mak) AS no_urut,
+    LEFT(id_mak, 4) + '-' + 
+    RIGHT(LEFT(id_mak, 10), 6) + '-' + 
+    RIGHT(LEFT(id_mak, 12), 2) + '-' + 
+    RIGHT(id_mak, 1) AS id_mak,
+    b41k1,
+    b41k3
+FROM MAK_B41
+WHERE b41k3 IS NOT NULL AND b41k3 != ''
+ORDER BY id_mak;</t>
+  </si>
+  <si>
+    <t>SELECT ROW_NUMBER() OVER (ORDER BY id_inti) AS no_urut, 
+ LEFT(id_inti, 4) + '-' + 
+    RIGHT(LEFT(id_inti, 10), 6) + '-' + 
+    RIGHT(LEFT(id_inti, 12), 2) + '-' + 
+    RIGHT(id_inti, 1) AS id_inti,
+    R456K3, jml_art_usia_sekolah,Catatan from inti_rt i 
 left JOIN (
     SELECT id_inti AS id_inti_art, COUNT(*) AS jml_art_usia_sekolah
         FROM INTI_ART 
@@ -238,21 +268,6 @@
 )jml ON jml.id_inti_art = i.id_inti
 where jml_art_usia_sekolah is not NULL and R456K3 =0
 order by id_inti</t>
-  </si>
-  <si>
-    <t>t2</t>
-  </si>
-  <si>
-    <t>T2. Rincian Lainnya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rincian 'Lainnya' di kuesioner makanan </t>
-  </si>
-  <si>
-    <t>select ROW_NUMBER() OVER (ORDER BY id_mak) AS no_urut,id_mak,
-b41k1, b41k3 from MAK_B41 
-where b41k3 is not null and b41k3 !=''
-order by id_mak</t>
   </si>
 </sst>
 </file>
@@ -618,10 +633,10 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="44" style="1" customWidth="1"/>
@@ -632,7 +647,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -652,7 +667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -672,7 +687,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -692,7 +707,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -712,7 +727,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -732,7 +747,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -752,7 +767,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -772,7 +787,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -792,7 +807,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="285" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -812,7 +827,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
@@ -826,27 +841,27 @@
         <v>1000</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
tambah form update token
</commit_message>
<xml_diff>
--- a/queries/query_list.xlsx
+++ b/queries/query_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2025\SERUTI\evaluasi-seruti-1800\queries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7065261-9CD8-4644-893D-D8FE1609777E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABBB51C-7BC6-4563-AFD9-7ABA6875F26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{764EDEE2-3088-4AC6-90FD-CA006F98D4D8}"/>
   </bookViews>
@@ -633,7 +633,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>